<commit_message>
✅ Tour & ChiTiet: Export to Excel
</commit_message>
<xml_diff>
--- a/storage/app/reports/bang-ke.xlsx
+++ b/storage/app/reports/bang-ke.xlsx
@@ -733,6 +733,9 @@
     <xf numFmtId="167" fontId="7" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,9 +753,6 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -10711,7 +10711,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="2E353D"/>
+        <a:sysClr val="windowText" lastClr="464646"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -10975,10 +10975,10 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="33" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="34" customWidth="1"/>
@@ -10992,8 +10992,8 @@
     <col min="10" max="10" width="12" style="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" style="33" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" style="40"/>
-    <col min="16" max="16384" width="9.140625" style="33"/>
+    <col min="13" max="15" width="0" style="40" hidden="1"/>
+    <col min="16" max="16384" width="9.140625" style="33" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
       <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="59" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="7"/>
@@ -11040,39 +11040,39 @@
       <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="36"/>
       <c r="N4" s="36"/>
       <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
       <c r="O5" s="36"/>
@@ -11280,38 +11280,38 @@
       <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="62"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="26"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="63" t="s">
+      <c r="I16" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
       <c r="L16" s="27"/>
       <c r="M16" s="36"/>
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
     </row>
     <row r="17" spans="1:15" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="62"/>
+      <c r="C17" s="63"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="64" t="s">
+      <c r="I17" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
       <c r="L17" s="27"/>
       <c r="M17" s="36"/>
       <c r="N17" s="36"/>
@@ -11410,226 +11410,226 @@
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
     </row>
-    <row r="24" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="41"/>
     </row>
-    <row r="25" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="41"/>
     </row>
-    <row r="26" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="41"/>
     </row>
-    <row r="27" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="41"/>
     </row>
-    <row r="28" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="41"/>
     </row>
-    <row r="29" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="41"/>
     </row>
-    <row r="30" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41"/>
     </row>
-    <row r="31" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="41"/>
     </row>
-    <row r="32" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="41"/>
     </row>
-    <row r="33" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="41"/>
     </row>
-    <row r="34" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="41"/>
     </row>
-    <row r="35" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="41"/>
     </row>
-    <row r="36" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="41"/>
     </row>
-    <row r="37" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="41"/>
     </row>
-    <row r="38" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="41"/>
     </row>
-    <row r="39" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="41"/>
     </row>
-    <row r="40" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="41"/>
     </row>
-    <row r="41" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="41"/>
     </row>
-    <row r="42" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="41"/>
     </row>
-    <row r="43" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="41"/>
     </row>
-    <row r="44" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="41"/>
     </row>
-    <row r="45" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="41"/>
     </row>
-    <row r="46" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="41"/>
     </row>
-    <row r="47" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="41"/>
     </row>
-    <row r="48" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="41"/>
     </row>
-    <row r="49" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="41"/>
     </row>
-    <row r="50" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="41"/>
     </row>
-    <row r="51" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="41"/>
     </row>
-    <row r="52" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="41"/>
     </row>
-    <row r="53" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="41"/>
     </row>
-    <row r="54" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="41"/>
     </row>
-    <row r="55" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="41"/>
     </row>
-    <row r="56" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="41"/>
     </row>
-    <row r="57" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="41"/>
     </row>
-    <row r="58" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="41"/>
     </row>
-    <row r="59" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="41"/>
     </row>
-    <row r="60" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="41"/>
     </row>
-    <row r="61" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="41"/>
     </row>
-    <row r="62" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="41"/>
     </row>
-    <row r="63" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="41"/>
     </row>
-    <row r="64" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="41"/>
     </row>
-    <row r="65" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="41"/>
     </row>
-    <row r="66" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="41"/>
     </row>
-    <row r="67" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="41"/>
     </row>
-    <row r="68" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="41"/>
     </row>
-    <row r="69" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="41"/>
     </row>
-    <row r="70" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="41"/>
     </row>
-    <row r="71" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="41"/>
     </row>
-    <row r="72" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="41"/>
     </row>
-    <row r="73" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="41"/>
     </row>
-    <row r="74" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="41"/>
     </row>
-    <row r="75" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="41"/>
     </row>
-    <row r="76" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="41"/>
     </row>
-    <row r="77" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="41"/>
     </row>
-    <row r="78" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="41"/>
     </row>
-    <row r="79" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="41"/>
     </row>
-    <row r="80" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="41"/>
     </row>
-    <row r="81" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="41"/>
     </row>
-    <row r="82" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="41"/>
     </row>
-    <row r="83" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="41"/>
     </row>
-    <row r="84" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="41"/>
     </row>
-    <row r="85" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="41"/>
     </row>
-    <row r="86" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="41"/>
     </row>
-    <row r="87" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="41"/>
     </row>
-    <row r="88" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="41"/>
     </row>
-    <row r="89" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="41"/>
     </row>
-    <row r="90" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="41"/>
     </row>
-    <row r="91" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="41"/>
     </row>
-    <row r="92" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="41"/>
     </row>
-    <row r="93" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="41"/>
     </row>
-    <row r="94" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="41"/>
     </row>
-    <row r="95" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="41"/>
     </row>
-    <row r="96" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="41"/>
     </row>
-    <row r="97" spans="2:2" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="41"/>
     </row>
   </sheetData>

</xml_diff>